<commit_message>
dailyscrum kevin & bram
</commit_message>
<xml_diff>
--- a/scrum/Dailyscrum.xlsx
+++ b/scrum/Dailyscrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fred\Documents\GitHub\project-appdev\AppDev05_2016\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bram\Documents\GitHub\project-appdev\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="989" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
   <si>
     <t>Datum</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>Aanmaken desktop mockups</t>
+  </si>
+  <si>
+    <t>statistiekenpagina en homepage mockup</t>
+  </si>
+  <si>
+    <t>UML class diagram</t>
+  </si>
+  <si>
+    <t>templates</t>
+  </si>
+  <si>
+    <t>mockup evenementen lijst</t>
   </si>
 </sst>
 </file>
@@ -297,7 +309,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -381,9 +393,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -421,7 +433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -493,7 +505,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -649,15 +661,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -668,7 +680,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -689,7 +701,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -700,7 +712,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -711,7 +723,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -739,15 +751,15 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7">
         <v>42426</v>
       </c>
@@ -758,7 +770,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -779,7 +791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -802,7 +814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -825,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -860,18 +872,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7">
         <v>42431</v>
       </c>
@@ -882,7 +894,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -903,7 +915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -926,7 +938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -949,7 +961,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -980,18 +992,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7">
         <v>42433</v>
       </c>
@@ -1002,7 +1014,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1023,7 +1035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1045,9 @@
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
         <v>29</v>
@@ -1042,7 +1056,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1050,12 +1064,16 @@
         <v>33</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1063,9 +1081,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
   </sheetData>
@@ -1082,18 +1104,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7">
         <v>42440</v>
       </c>
@@ -1104,7 +1126,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1125,7 +1147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1133,12 +1155,16 @@
         <v>34</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1148,14 +1174,18 @@
       <c r="C4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="G4" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1182,18 +1212,18 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="25.28515625"/>
-    <col min="7" max="7" width="38.7109375"/>
-    <col min="8" max="9" width="25.28515625"/>
-    <col min="10" max="1025" width="8.7109375"/>
+    <col min="1" max="6" width="25.33203125"/>
+    <col min="7" max="7" width="38.6640625"/>
+    <col min="8" max="9" width="25.33203125"/>
+    <col min="10" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1204,7 +1234,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1225,7 +1255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="121.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="121.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1235,14 +1265,18 @@
       <c r="C3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="G3" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1255,7 +1289,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="104.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="104.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>

</xml_diff>